<commit_message>
small experiments and cleanup
</commit_message>
<xml_diff>
--- a/SpeedDATA/Optimization.xlsx
+++ b/SpeedDATA/Optimization.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="65">
   <si>
     <t>Speed - Analyser - Results:</t>
   </si>
@@ -589,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V46"/>
+  <dimension ref="A1:V75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1185,7 @@
         <v>2</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:B45" si="0">B3</f>
+        <f>B3</f>
         <v>5.8110944527736095</v>
       </c>
       <c r="C26">
@@ -1198,19 +1198,19 @@
         <v>3</v>
       </c>
       <c r="B27" s="1">
-        <f t="shared" si="0"/>
+        <f>B4</f>
         <v>1.7391304347826039E-2</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ref="C27:C45" si="1">F4</f>
+        <f t="shared" ref="C27:C45" si="0">F4</f>
         <v>2.6564682712345647E-3</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E43" si="2">C27</f>
+        <f t="shared" ref="E27:E43" si="1">C27</f>
         <v>2.6564682712345647E-3</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:F45" si="3">ROUND(E27*100,1)</f>
+        <f t="shared" ref="F27:F45" si="2">ROUND(E27*100,1)</f>
         <v>0.3</v>
       </c>
       <c r="G27">
@@ -1231,7 +1231,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1">
-        <f t="shared" si="0"/>
+        <f>B5</f>
         <v>2.1389305347326297E-2</v>
       </c>
       <c r="C28" s="1">
@@ -1239,11 +1239,11 @@
         <v>3.2671506324379162E-3</v>
       </c>
       <c r="E28">
+        <f t="shared" si="1"/>
+        <v>3.2671506324379162E-3</v>
+      </c>
+      <c r="F28">
         <f t="shared" si="2"/>
-        <v>3.2671506324379162E-3</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
       <c r="G28">
@@ -1264,7 +1264,7 @@
         <v>5</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f>B6</f>
         <v>3.190304847576209</v>
       </c>
       <c r="C29">
@@ -1277,7 +1277,7 @@
         <v>6</v>
       </c>
       <c r="B30" s="1">
-        <f t="shared" si="0"/>
+        <f>B7</f>
         <v>2.3483889829242816E-5</v>
       </c>
       <c r="C30" s="1">
@@ -1285,11 +1285,11 @@
         <v>4.3707303228520956E-4</v>
       </c>
       <c r="E30">
+        <f t="shared" si="1"/>
+        <v>4.3707303228520956E-4</v>
+      </c>
+      <c r="F30">
         <f t="shared" si="2"/>
-        <v>4.3707303228520956E-4</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G30">
@@ -1310,19 +1310,19 @@
         <v>7</v>
       </c>
       <c r="B31" s="1">
-        <f t="shared" si="0"/>
+        <f>B8</f>
         <v>1.2702139866037818E-3</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ref="C31:C34" si="4">K8</f>
+        <f t="shared" ref="C31:C34" si="3">K8</f>
         <v>2.3640729147207884E-2</v>
       </c>
       <c r="E31">
+        <f t="shared" si="1"/>
+        <v>2.3640729147207884E-2</v>
+      </c>
+      <c r="F31">
         <f t="shared" si="2"/>
-        <v>2.3640729147207884E-2</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="3"/>
         <v>2.4</v>
       </c>
       <c r="G31">
@@ -1343,19 +1343,19 @@
         <v>8</v>
       </c>
       <c r="B32" s="1">
-        <f t="shared" si="0"/>
+        <f>B9</f>
         <v>4.2641236350175852E-4</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>7.9362212169612166E-3</v>
       </c>
       <c r="E32">
+        <f t="shared" si="1"/>
+        <v>7.9362212169612166E-3</v>
+      </c>
+      <c r="F32">
         <f t="shared" si="2"/>
-        <v>7.9362212169612166E-3</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
       <c r="G32">
@@ -1376,19 +1376,19 @@
         <v>9</v>
       </c>
       <c r="B33" s="1">
-        <f t="shared" si="0"/>
+        <f>B10</f>
         <v>2.4415040570250832E-2</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.45440324805637222</v>
       </c>
       <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0.45440324805637222</v>
+      </c>
+      <c r="F33">
         <f t="shared" si="2"/>
-        <v>0.45440324805637222</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="3"/>
         <v>45.4</v>
       </c>
       <c r="G33">
@@ -1409,19 +1409,19 @@
         <v>10</v>
       </c>
       <c r="B34" s="1">
-        <f t="shared" si="0"/>
+        <f>B11</f>
         <v>4.7926302993023508E-5</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>8.9198572841609576E-4</v>
       </c>
       <c r="E34">
+        <f t="shared" si="1"/>
+        <v>8.9198572841609576E-4</v>
+      </c>
+      <c r="F34">
         <f t="shared" si="2"/>
-        <v>8.9198572841609576E-4</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="G34">
@@ -1442,11 +1442,11 @@
         <v>11</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f>B12</f>
         <v>2.3845077461269311</v>
       </c>
       <c r="C35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.36422622728070714</v>
       </c>
     </row>
@@ -1455,7 +1455,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="1">
-        <f t="shared" si="0"/>
+        <f>B13</f>
         <v>4.5911125611869939E-4</v>
       </c>
       <c r="C36" s="1">
@@ -1463,11 +1463,11 @@
         <v>8.5202004223589953E-3</v>
       </c>
       <c r="E36">
+        <f t="shared" si="1"/>
+        <v>8.5202004223589953E-3</v>
+      </c>
+      <c r="F36">
         <f t="shared" si="2"/>
-        <v>8.5202004223589953E-3</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
       <c r="G36">
@@ -1488,7 +1488,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="5">
-        <f t="shared" si="0"/>
+        <f>B14</f>
         <v>1.9167229959915971E-2</v>
       </c>
       <c r="C37" s="5">
@@ -1501,7 +1501,7 @@
         <v>14</v>
       </c>
       <c r="B38" s="5">
-        <f t="shared" si="0"/>
+        <f>B15</f>
         <v>1.432999797061249E-2</v>
       </c>
       <c r="C38" s="5">
@@ -1514,7 +1514,7 @@
         <v>15</v>
       </c>
       <c r="B39" s="1">
-        <f t="shared" si="0"/>
+        <f>B16</f>
         <v>2.4747053833481179E-5</v>
       </c>
       <c r="C39" s="1">
@@ -1522,11 +1522,11 @@
         <v>4.8893057542579322E-4</v>
       </c>
       <c r="E39">
+        <f t="shared" si="1"/>
+        <v>4.8893057542579322E-4</v>
+      </c>
+      <c r="F39">
         <f t="shared" si="2"/>
-        <v>4.8893057542579322E-4</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G39">
@@ -1547,19 +1547,19 @@
         <v>16</v>
       </c>
       <c r="B40" s="1">
-        <f t="shared" si="0"/>
+        <f>B17</f>
         <v>2.7101014682564492E-3</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" ref="C40:C42" si="5">V17</f>
+        <f t="shared" ref="C40:C42" si="4">V17</f>
         <v>5.3543806840723927E-2</v>
       </c>
       <c r="E40">
+        <f t="shared" si="1"/>
+        <v>5.3543806840723927E-2</v>
+      </c>
+      <c r="F40">
         <f t="shared" si="2"/>
-        <v>5.3543806840723927E-2</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="3"/>
         <v>5.4</v>
       </c>
       <c r="G40">
@@ -1580,19 +1580,19 @@
         <v>17</v>
       </c>
       <c r="B41" s="1">
-        <f t="shared" si="0"/>
+        <f>B18</f>
         <v>5.7613346154347586E-3</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.11382739406878334</v>
       </c>
       <c r="E41">
+        <f t="shared" si="1"/>
+        <v>0.11382739406878334</v>
+      </c>
+      <c r="F41">
         <f t="shared" si="2"/>
-        <v>0.11382739406878334</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="3"/>
         <v>11.4</v>
       </c>
       <c r="G41">
@@ -1613,19 +1613,19 @@
         <v>18</v>
       </c>
       <c r="B42" s="1">
-        <f t="shared" si="0"/>
+        <f>B19</f>
         <v>5.0055161456185326E-3</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.8894595932436213E-2</v>
       </c>
       <c r="E42">
+        <f t="shared" si="1"/>
+        <v>9.8894595932436213E-2</v>
+      </c>
+      <c r="F42">
         <f t="shared" si="2"/>
-        <v>9.8894595932436213E-2</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="3"/>
         <v>9.9</v>
       </c>
       <c r="G42">
@@ -1646,7 +1646,7 @@
         <v>19</v>
       </c>
       <c r="B43" s="1">
-        <f t="shared" si="0"/>
+        <f>B20</f>
         <v>4.7784418023759951E-3</v>
       </c>
       <c r="C43" s="1">
@@ -1654,11 +1654,11 @@
         <v>8.8951299440978876E-2</v>
       </c>
       <c r="E43">
+        <f t="shared" si="1"/>
+        <v>8.8951299440978876E-2</v>
+      </c>
+      <c r="F43">
         <f t="shared" si="2"/>
-        <v>8.8951299440978876E-2</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="3"/>
         <v>8.9</v>
       </c>
       <c r="G43">
@@ -1679,11 +1679,11 @@
         <v>20</v>
       </c>
       <c r="B44" s="1">
-        <f t="shared" si="0"/>
+        <f>B21</f>
         <v>6.946526736631679E-3</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.0610606025908196E-3</v>
       </c>
       <c r="E44">
@@ -1691,7 +1691,7 @@
         <v>1.0610606025908196E-3</v>
       </c>
       <c r="F44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="G44">
@@ -1712,11 +1712,11 @@
         <v>21</v>
       </c>
       <c r="B45" s="1">
-        <f t="shared" si="0"/>
+        <f>B22</f>
         <v>0.18190904547726083</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.7786047434752343E-2</v>
       </c>
       <c r="E45">
@@ -1724,7 +1724,7 @@
         <v>2.7786047434752343E-2</v>
       </c>
       <c r="F45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>2.8</v>
       </c>
       <c r="G45">
@@ -1763,6 +1763,179 @@
       <c r="J46">
         <f>SUM(J25:J45)</f>
         <v>0.99863280610406979</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>0.85701299881828896</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56">
+        <v>6.5936733024270504</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57">
+        <v>1.3453322425233999E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58">
+        <v>1.59076447595673E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59">
+        <v>3.3826924825015898</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1.21274555598719E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61">
+        <v>1.2760482086348801E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B62" s="3">
+        <v>4.1379944520222498E-4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63">
+        <v>2.27629675483948E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>48</v>
+      </c>
+      <c r="B64" s="3">
+        <v>3.39835293161247E-5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B65">
+        <v>2.9669120989000999</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" s="3">
+        <v>3.5983447614097502E-4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>51</v>
+      </c>
+      <c r="B67">
+        <v>2.1312862749801698E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>52</v>
+      </c>
+      <c r="B68">
+        <v>1.64264438358355E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1.45266510738393E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>54</v>
+      </c>
+      <c r="B70">
+        <v>3.0292732009941999E-3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>55</v>
+      </c>
+      <c r="B71">
+        <v>7.5192078310643701E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72">
+        <v>4.7684731690089202E-3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73">
+        <v>4.8371082635321003E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74">
+        <v>1.48168348331969E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75">
+        <v>0.19380056358512801</v>
       </c>
     </row>
   </sheetData>
@@ -3045,7 +3218,7 @@
         <v>2.643678160919536E-2</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N3:N22" si="1">_xlfn.STDEV.S(B4:K4)</f>
+        <f t="shared" ref="N4:N22" si="1">_xlfn.STDEV.S(B4:K4)</f>
         <v>4.3404480338240263E-3</v>
       </c>
     </row>
@@ -3931,11 +4104,11 @@
         <v>1.07096451774112</v>
       </c>
       <c r="M2" s="4">
-        <f>SUM(B2:K2)/10</f>
+        <f t="shared" ref="M2:M22" si="0">SUM(B2:K2)/10</f>
         <v>0.97351324337830825</v>
       </c>
       <c r="N2">
-        <f>_xlfn.STDEV.S(B2:K2)</f>
+        <f t="shared" ref="N2:N22" si="1">_xlfn.STDEV.S(B2:K2)</f>
         <v>5.5115186464548396E-2</v>
       </c>
     </row>
@@ -3974,11 +4147,11 @@
         <v>11.5297351324337</v>
       </c>
       <c r="M3" s="4">
-        <f>SUM(B3:K3)/10</f>
+        <f t="shared" si="0"/>
         <v>10.630234882558668</v>
       </c>
       <c r="N3">
-        <f>_xlfn.STDEV.S(B3:K3)</f>
+        <f t="shared" si="1"/>
         <v>0.46154860123130514</v>
       </c>
     </row>
@@ -4017,11 +4190,11 @@
         <v>2.6986506746626601E-2</v>
       </c>
       <c r="M4" s="4">
-        <f>SUM(B4:K4)/10</f>
+        <f t="shared" si="0"/>
         <v>2.108945527236377E-2</v>
       </c>
       <c r="N4">
-        <f>_xlfn.STDEV.S(B4:K4)</f>
+        <f t="shared" si="1"/>
         <v>4.5242032841627169E-3</v>
       </c>
     </row>
@@ -4060,11 +4233,11 @@
         <v>2.64867566216891E-2</v>
       </c>
       <c r="M5" s="4">
-        <f>SUM(B5:K5)/10</f>
+        <f t="shared" si="0"/>
         <v>1.9940029985007438E-2</v>
       </c>
       <c r="N5">
-        <f>_xlfn.STDEV.S(B5:K5)</f>
+        <f t="shared" si="1"/>
         <v>4.7084489625205785E-3</v>
       </c>
     </row>
@@ -4103,11 +4276,11 @@
         <v>4.2023988005996999</v>
       </c>
       <c r="M6" s="4">
-        <f>SUM(B6:K6)/10</f>
+        <f t="shared" si="0"/>
         <v>3.9480759620189865</v>
       </c>
       <c r="N6">
-        <f>_xlfn.STDEV.S(B6:K6)</f>
+        <f t="shared" si="1"/>
         <v>0.25434498817492679</v>
       </c>
     </row>
@@ -4146,11 +4319,11 @@
         <v>3.4475031458466201E-5</v>
       </c>
       <c r="M7" s="8">
-        <f>SUM(B7:K7)/10</f>
+        <f t="shared" si="0"/>
         <v>2.3696557132502907E-5</v>
       </c>
       <c r="N7">
-        <f>_xlfn.STDEV.S(B7:K7)</f>
+        <f t="shared" si="1"/>
         <v>1.5741548309798617E-5</v>
       </c>
     </row>
@@ -4189,11 +4362,11 @@
         <v>1.7797734990433101E-3</v>
       </c>
       <c r="M8" s="8">
-        <f>SUM(B8:K8)/10</f>
+        <f t="shared" si="0"/>
         <v>1.5764675617321959E-3</v>
       </c>
       <c r="N8">
-        <f>_xlfn.STDEV.S(B8:K8)</f>
+        <f t="shared" si="1"/>
         <v>2.7491870783815346E-4</v>
       </c>
     </row>
@@ -4232,11 +4405,11 @@
         <v>5.4729112440315096E-4</v>
       </c>
       <c r="M9" s="8">
-        <f>SUM(B9:K9)/10</f>
+        <f t="shared" si="0"/>
         <v>5.5106275085762602E-4</v>
       </c>
       <c r="N9">
-        <f>_xlfn.STDEV.S(B9:K9)</f>
+        <f t="shared" si="1"/>
         <v>8.1048698850371927E-5</v>
       </c>
     </row>
@@ -4275,11 +4448,11 @@
         <v>3.34407805147122E-2</v>
       </c>
       <c r="M10" s="8">
-        <f>SUM(B10:K10)/10</f>
+        <f t="shared" si="0"/>
         <v>3.2880417748991864E-2</v>
       </c>
       <c r="N10">
-        <f>_xlfn.STDEV.S(B10:K10)</f>
+        <f t="shared" si="1"/>
         <v>1.853834293308814E-3</v>
       </c>
     </row>
@@ -4318,11 +4491,11 @@
         <v>9.4806336510781995E-5</v>
       </c>
       <c r="M11" s="8">
-        <f>SUM(B11:K11)/10</f>
+        <f t="shared" si="0"/>
         <v>6.8149287271854621E-5</v>
       </c>
       <c r="N11">
-        <f>_xlfn.STDEV.S(B11:K11)</f>
+        <f t="shared" si="1"/>
         <v>2.9022546386049809E-5</v>
       </c>
     </row>
@@ -4361,11 +4534,11 @@
         <v>7.0014992503748097</v>
       </c>
       <c r="M12" s="4">
-        <f>SUM(B12:K12)/10</f>
+        <f t="shared" si="0"/>
         <v>6.3855572213892984</v>
       </c>
       <c r="N12">
-        <f>_xlfn.STDEV.S(B12:K12)</f>
+        <f t="shared" si="1"/>
         <v>0.27270957752062625</v>
       </c>
     </row>
@@ -4404,11 +4577,11 @@
         <v>8.3171371810507105E-4</v>
       </c>
       <c r="M13" s="8">
-        <f>SUM(B13:K13)/10</f>
+        <f t="shared" si="0"/>
         <v>7.2745857066157361E-4</v>
       </c>
       <c r="N13">
-        <f>_xlfn.STDEV.S(B13:K13)</f>
+        <f t="shared" si="1"/>
         <v>7.0794582642355518E-5</v>
       </c>
     </row>
@@ -4447,11 +4620,11 @@
         <v>5.9349022413176397E-2</v>
       </c>
       <c r="M14" s="8">
-        <f>SUM(B14:K14)/10</f>
+        <f t="shared" si="0"/>
         <v>5.6325677229999371E-2</v>
       </c>
       <c r="N14">
-        <f>_xlfn.STDEV.S(B14:K14)</f>
+        <f t="shared" si="1"/>
         <v>2.022325574901911E-3</v>
       </c>
     </row>
@@ -4490,11 +4663,11 @@
         <v>2.4559256370366801E-2</v>
       </c>
       <c r="M15" s="8">
-        <f>SUM(B15:K15)/10</f>
+        <f t="shared" si="0"/>
         <v>2.2901450917909391E-2</v>
       </c>
       <c r="N15">
-        <f>_xlfn.STDEV.S(B15:K15)</f>
+        <f t="shared" si="1"/>
         <v>1.2883601340495806E-3</v>
       </c>
     </row>
@@ -4533,11 +4706,11 @@
         <v>3.0165782521945601E-5</v>
       </c>
       <c r="M16" s="8">
-        <f>SUM(B16:K16)/10</f>
+        <f t="shared" si="0"/>
         <v>2.3760752465257153E-5</v>
       </c>
       <c r="N16">
-        <f>_xlfn.STDEV.S(B16:K16)</f>
+        <f t="shared" si="1"/>
         <v>1.6093702593467367E-5</v>
       </c>
     </row>
@@ -4576,11 +4749,11 @@
         <v>4.3050881056319497E-3</v>
       </c>
       <c r="M17" s="8">
-        <f>SUM(B17:K17)/10</f>
+        <f t="shared" si="0"/>
         <v>3.8076697879026455E-3</v>
       </c>
       <c r="N17">
-        <f>_xlfn.STDEV.S(B17:K17)</f>
+        <f t="shared" si="1"/>
         <v>2.9691253246079137E-4</v>
       </c>
     </row>
@@ -4619,11 +4792,11 @@
         <v>1.1962887468703E-2</v>
       </c>
       <c r="M18" s="8">
-        <f>SUM(B18:K18)/10</f>
+        <f t="shared" si="0"/>
         <v>1.1310349534762449E-2</v>
       </c>
       <c r="N18">
-        <f>_xlfn.STDEV.S(B18:K18)</f>
+        <f t="shared" si="1"/>
         <v>9.631949587563534E-4</v>
       </c>
     </row>
@@ -4662,11 +4835,11 @@
         <v>6.4727150497088997E-3</v>
       </c>
       <c r="M19" s="8">
-        <f>SUM(B19:K19)/10</f>
+        <f t="shared" si="0"/>
         <v>6.1278189330018756E-3</v>
       </c>
       <c r="N19">
-        <f>_xlfn.STDEV.S(B19:K19)</f>
+        <f t="shared" si="1"/>
         <v>4.1751085138578967E-4</v>
       </c>
     </row>
@@ -4705,11 +4878,11 @@
         <v>3.4630318335193498E-2</v>
       </c>
       <c r="M20" s="8">
-        <f>SUM(B20:K20)/10</f>
+        <f t="shared" si="0"/>
         <v>3.3270817099109368E-2</v>
       </c>
       <c r="N20">
-        <f>_xlfn.STDEV.S(B20:K20)</f>
+        <f t="shared" si="1"/>
         <v>9.2212907510264821E-4</v>
       </c>
     </row>
@@ -4748,11 +4921,11 @@
         <v>3.5982008995502197E-2</v>
       </c>
       <c r="M21" s="4">
-        <f>SUM(B21:K21)/10</f>
+        <f t="shared" si="0"/>
         <v>2.9735132433783069E-2</v>
       </c>
       <c r="N21">
-        <f>_xlfn.STDEV.S(B21:K21)</f>
+        <f t="shared" si="1"/>
         <v>6.5084872882180079E-3</v>
       </c>
     </row>
@@ -4791,11 +4964,11 @@
         <v>0.22538730634682599</v>
       </c>
       <c r="M22" s="4">
-        <f>SUM(B22:K22)/10</f>
+        <f t="shared" si="0"/>
         <v>0.21344327836081906</v>
       </c>
       <c r="N22">
-        <f>_xlfn.STDEV.S(B22:K22)</f>
+        <f t="shared" si="1"/>
         <v>1.4388889127790828E-2</v>
       </c>
     </row>
@@ -4893,11 +5066,11 @@
         <v>0.776111944027986</v>
       </c>
       <c r="M2" s="4">
-        <f>SUM(B2:K2)/10</f>
+        <f t="shared" ref="M2:M22" si="0">SUM(B2:K2)/10</f>
         <v>0.72143928035981963</v>
       </c>
       <c r="N2">
-        <f>_xlfn.STDEV.S(B2:K2)</f>
+        <f t="shared" ref="N2:N22" si="1">_xlfn.STDEV.S(B2:K2)</f>
         <v>3.8695564647442199E-2</v>
       </c>
     </row>
@@ -4936,11 +5109,11 @@
         <v>5.4717641179410297</v>
       </c>
       <c r="M3" s="4">
-        <f>SUM(B3:K3)/10</f>
+        <f t="shared" si="0"/>
         <v>5.3829085457271315</v>
       </c>
       <c r="N3">
-        <f>_xlfn.STDEV.S(B3:K3)</f>
+        <f t="shared" si="1"/>
         <v>0.20809801630341235</v>
       </c>
     </row>
@@ -4979,11 +5152,11 @@
         <v>1.9990004997501198E-2</v>
       </c>
       <c r="M4" s="4">
-        <f>SUM(B4:K4)/10</f>
+        <f t="shared" si="0"/>
         <v>1.889055472263863E-2</v>
       </c>
       <c r="N4">
-        <f>_xlfn.STDEV.S(B4:K4)</f>
+        <f t="shared" si="1"/>
         <v>4.9180197382925651E-3</v>
       </c>
     </row>
@@ -5022,11 +5195,11 @@
         <v>1.24937531234382E-2</v>
       </c>
       <c r="M5" s="4">
-        <f>SUM(B5:K5)/10</f>
+        <f t="shared" si="0"/>
         <v>2.0089955022488708E-2</v>
       </c>
       <c r="N5">
-        <f>_xlfn.STDEV.S(B5:K5)</f>
+        <f t="shared" si="1"/>
         <v>6.437967932192229E-3</v>
       </c>
     </row>
@@ -5065,11 +5238,11 @@
         <v>2.7741129435282299</v>
       </c>
       <c r="M6" s="4">
-        <f>SUM(B6:K6)/10</f>
+        <f t="shared" si="0"/>
         <v>2.729385307346321</v>
       </c>
       <c r="N6">
-        <f>_xlfn.STDEV.S(B6:K6)</f>
+        <f t="shared" si="1"/>
         <v>0.20463359033073966</v>
       </c>
     </row>
@@ -5108,11 +5281,11 @@
         <v>8.5908438785941895E-6</v>
       </c>
       <c r="M7" s="8">
-        <f>SUM(B7:K7)/10</f>
+        <f t="shared" si="0"/>
         <v>1.7269565108197846E-5</v>
       </c>
       <c r="N7">
-        <f>_xlfn.STDEV.S(B7:K7)</f>
+        <f t="shared" si="1"/>
         <v>1.3770520719315767E-5</v>
       </c>
     </row>
@@ -5151,11 +5324,11 @@
         <v>1.0394921093098901E-3</v>
       </c>
       <c r="M8" s="8">
-        <f>SUM(B8:K8)/10</f>
+        <f t="shared" si="0"/>
         <v>1.0566890614612113E-3</v>
       </c>
       <c r="N8">
-        <f>_xlfn.STDEV.S(B8:K8)</f>
+        <f t="shared" si="1"/>
         <v>1.4671138541419329E-4</v>
       </c>
     </row>
@@ -5194,11 +5367,11 @@
         <v>3.9517881841533202E-4</v>
       </c>
       <c r="M9" s="8">
-        <f>SUM(B9:K9)/10</f>
+        <f t="shared" si="0"/>
         <v>4.0616683631354886E-4</v>
       </c>
       <c r="N9">
-        <f>_xlfn.STDEV.S(B9:K9)</f>
+        <f t="shared" si="1"/>
         <v>4.9359355512166932E-5</v>
       </c>
     </row>
@@ -5237,11 +5410,11 @@
         <v>2.2203036004226601E-2</v>
       </c>
       <c r="M10" s="8">
-        <f>SUM(B10:K10)/10</f>
+        <f t="shared" si="0"/>
         <v>2.2245852587946258E-2</v>
       </c>
       <c r="N10">
-        <f>_xlfn.STDEV.S(B10:K10)</f>
+        <f t="shared" si="1"/>
         <v>1.8066758628016918E-3</v>
       </c>
     </row>
@@ -5280,11 +5453,11 @@
         <v>2.14771096964854E-5</v>
       </c>
       <c r="M11" s="8">
-        <f>SUM(B11:K11)/10</f>
+        <f t="shared" si="0"/>
         <v>3.4290858429736784E-5</v>
       </c>
       <c r="N11">
-        <f>_xlfn.STDEV.S(B11:K11)</f>
+        <f t="shared" si="1"/>
         <v>1.5976527387454177E-5</v>
       </c>
     </row>
@@ -5323,11 +5496,11 @@
         <v>2.4727636181908998</v>
       </c>
       <c r="M12" s="4">
-        <f>SUM(B12:K12)/10</f>
+        <f t="shared" si="0"/>
         <v>2.3995502248875531</v>
       </c>
       <c r="N12">
-        <f>_xlfn.STDEV.S(B12:K12)</f>
+        <f t="shared" si="1"/>
         <v>4.98021609552394E-2</v>
       </c>
     </row>
@@ -5366,11 +5539,11 @@
         <v>3.3504578959124402E-4</v>
       </c>
       <c r="M13" s="8">
-        <f>SUM(B13:K13)/10</f>
+        <f t="shared" si="0"/>
         <v>3.936694098224289E-4</v>
       </c>
       <c r="N13">
-        <f>_xlfn.STDEV.S(B13:K13)</f>
+        <f t="shared" si="1"/>
         <v>6.4510959806110787E-5</v>
       </c>
     </row>
@@ -5409,11 +5582,11 @@
         <v>2.08802254256799E-2</v>
       </c>
       <c r="M14" s="8">
-        <f>SUM(B14:K14)/10</f>
+        <f t="shared" si="0"/>
         <v>2.0575917632189182E-2</v>
       </c>
       <c r="N14">
-        <f>_xlfn.STDEV.S(B14:K14)</f>
+        <f t="shared" si="1"/>
         <v>5.4033861727210573E-4</v>
       </c>
     </row>
@@ -5452,11 +5625,11 @@
         <v>1.65847665847665E-2</v>
       </c>
       <c r="M15" s="8">
-        <f>SUM(B15:K15)/10</f>
+        <f t="shared" si="0"/>
         <v>1.6090631890573311E-2</v>
       </c>
       <c r="N15">
-        <f>_xlfn.STDEV.S(B15:K15)</f>
+        <f t="shared" si="1"/>
         <v>5.4429475841282621E-4</v>
       </c>
     </row>
@@ -5495,11 +5668,11 @@
         <v>8.5909176818267697E-6</v>
       </c>
       <c r="M16" s="8">
-        <f>SUM(B16:K16)/10</f>
+        <f t="shared" si="0"/>
         <v>1.18771868461407E-5</v>
       </c>
       <c r="N16">
-        <f>_xlfn.STDEV.S(B16:K16)</f>
+        <f t="shared" si="1"/>
         <v>9.6732937016095623E-6</v>
       </c>
     </row>
@@ -5538,11 +5711,11 @@
         <v>2.5729798457071098E-3</v>
       </c>
       <c r="M17" s="8">
-        <f>SUM(B17:K17)/10</f>
+        <f t="shared" si="0"/>
         <v>2.5228993214218782E-3</v>
       </c>
       <c r="N17">
-        <f>_xlfn.STDEV.S(B17:K17)</f>
+        <f t="shared" si="1"/>
         <v>1.1757852364665606E-4</v>
       </c>
     </row>
@@ -5581,11 +5754,11 @@
         <v>8.4405766223948006E-3</v>
       </c>
       <c r="M18" s="8">
-        <f>SUM(B18:K18)/10</f>
+        <f t="shared" si="0"/>
         <v>7.8408439187412464E-3</v>
       </c>
       <c r="N18">
-        <f>_xlfn.STDEV.S(B18:K18)</f>
+        <f t="shared" si="1"/>
         <v>4.4485629236075739E-4</v>
       </c>
     </row>
@@ -5624,11 +5797,11 @@
         <v>4.63050463050463E-3</v>
       </c>
       <c r="M19" s="8">
-        <f>SUM(B19:K19)/10</f>
+        <f t="shared" si="0"/>
         <v>4.879230471747471E-3</v>
       </c>
       <c r="N19">
-        <f>_xlfn.STDEV.S(B19:K19)</f>
+        <f t="shared" si="1"/>
         <v>2.7447164565851725E-4</v>
       </c>
     </row>
@@ -5667,11 +5840,11 @@
         <v>4.2653906290269902E-3</v>
       </c>
       <c r="M20" s="8">
-        <f>SUM(B20:K20)/10</f>
+        <f t="shared" si="0"/>
         <v>4.4334965423485024E-3</v>
       </c>
       <c r="N20">
-        <f>_xlfn.STDEV.S(B20:K20)</f>
+        <f t="shared" si="1"/>
         <v>1.6037788424864253E-4</v>
       </c>
     </row>
@@ -5710,11 +5883,11 @@
         <v>4.99750124937531E-3</v>
       </c>
       <c r="M21" s="4">
-        <f>SUM(B21:K21)/10</f>
+        <f t="shared" si="0"/>
         <v>3.3983008495752079E-3</v>
       </c>
       <c r="N21">
-        <f>_xlfn.STDEV.S(B21:K21)</f>
+        <f t="shared" si="1"/>
         <v>1.7755005956320809E-3</v>
       </c>
     </row>
@@ -5753,11 +5926,11 @@
         <v>0.18040979510244801</v>
       </c>
       <c r="M22" s="4">
-        <f>SUM(B22:K22)/10</f>
+        <f t="shared" si="0"/>
         <v>0.2032483758120934</v>
       </c>
       <c r="N22">
-        <f>_xlfn.STDEV.S(B22:K22)</f>
+        <f t="shared" si="1"/>
         <v>4.3304661203375068E-2</v>
       </c>
     </row>
@@ -5855,11 +6028,11 @@
         <v>0.74712643678160895</v>
       </c>
       <c r="M2" s="4">
-        <f>SUM(B2:K2)/10</f>
+        <f t="shared" ref="M2:M22" si="0">SUM(B2:K2)/10</f>
         <v>0.73568215892053934</v>
       </c>
       <c r="N2">
-        <f>_xlfn.STDEV.S(B2:K2)</f>
+        <f t="shared" ref="N2:N22" si="1">_xlfn.STDEV.S(B2:K2)</f>
         <v>4.7873784000195437E-2</v>
       </c>
     </row>
@@ -5898,11 +6071,11 @@
         <v>5.9205397301349301</v>
       </c>
       <c r="M3" s="4">
-        <f>SUM(B3:K3)/10</f>
+        <f t="shared" si="0"/>
         <v>5.8110944527736095</v>
       </c>
       <c r="N3">
-        <f>_xlfn.STDEV.S(B3:K3)</f>
+        <f t="shared" si="1"/>
         <v>0.27718572590080026</v>
       </c>
     </row>
@@ -5941,11 +6114,11 @@
         <v>1.09945027486256E-2</v>
       </c>
       <c r="M4" s="4">
-        <f>SUM(B4:K4)/10</f>
+        <f t="shared" si="0"/>
         <v>1.7391304347826039E-2</v>
       </c>
       <c r="N4">
-        <f>_xlfn.STDEV.S(B4:K4)</f>
+        <f t="shared" si="1"/>
         <v>4.7222787645915835E-3</v>
       </c>
     </row>
@@ -5984,11 +6157,11 @@
         <v>1.64917541229385E-2</v>
       </c>
       <c r="M5" s="4">
-        <f>SUM(B5:K5)/10</f>
+        <f t="shared" si="0"/>
         <v>2.1389305347326297E-2</v>
       </c>
       <c r="N5">
-        <f>_xlfn.STDEV.S(B5:K5)</f>
+        <f t="shared" si="1"/>
         <v>3.9477096767879067E-3</v>
       </c>
     </row>
@@ -6027,11 +6200,11 @@
         <v>3.3238380809595198</v>
       </c>
       <c r="M6" s="4">
-        <f>SUM(B6:K6)/10</f>
+        <f t="shared" si="0"/>
         <v>3.190304847576209</v>
       </c>
       <c r="N6">
-        <f>_xlfn.STDEV.S(B6:K6)</f>
+        <f t="shared" si="1"/>
         <v>0.22484359859382777</v>
       </c>
     </row>
@@ -6070,11 +6243,11 @@
         <v>8.4318098458243506E-6</v>
       </c>
       <c r="M7" s="8">
-        <f>SUM(B7:K7)/10</f>
+        <f t="shared" si="0"/>
         <v>2.3483889829242816E-5</v>
       </c>
       <c r="N7">
-        <f>_xlfn.STDEV.S(B7:K7)</f>
+        <f t="shared" si="1"/>
         <v>1.6555593812341695E-5</v>
       </c>
     </row>
@@ -6113,11 +6286,11 @@
         <v>1.1931010931841401E-3</v>
       </c>
       <c r="M8" s="8">
-        <f>SUM(B8:K8)/10</f>
+        <f t="shared" si="0"/>
         <v>1.2702139866037818E-3</v>
       </c>
       <c r="N8">
-        <f>_xlfn.STDEV.S(B8:K8)</f>
+        <f t="shared" si="1"/>
         <v>9.3890700290286436E-5</v>
       </c>
     </row>
@@ -6156,11 +6329,11 @@
         <v>4.1737458736830501E-4</v>
       </c>
       <c r="M9" s="8">
-        <f>SUM(B9:K9)/10</f>
+        <f t="shared" si="0"/>
         <v>4.2641236350175852E-4</v>
       </c>
       <c r="N9">
-        <f>_xlfn.STDEV.S(B9:K9)</f>
+        <f t="shared" si="1"/>
         <v>4.8255078345713941E-5</v>
       </c>
     </row>
@@ -6199,11 +6372,11 @@
         <v>2.6214496810667901E-2</v>
       </c>
       <c r="M10" s="8">
-        <f>SUM(B10:K10)/10</f>
+        <f t="shared" si="0"/>
         <v>2.4415040570250832E-2</v>
       </c>
       <c r="N10">
-        <f>_xlfn.STDEV.S(B10:K10)</f>
+        <f t="shared" si="1"/>
         <v>1.7060379085354991E-3</v>
       </c>
     </row>
@@ -6242,11 +6415,11 @@
         <v>5.4806763997858301E-5</v>
       </c>
       <c r="M11" s="8">
-        <f>SUM(B11:K11)/10</f>
+        <f t="shared" si="0"/>
         <v>4.7926302993023508E-5</v>
       </c>
       <c r="N11">
-        <f>_xlfn.STDEV.S(B11:K11)</f>
+        <f t="shared" si="1"/>
         <v>1.6920267109356505E-5</v>
       </c>
     </row>
@@ -6285,11 +6458,11 @@
         <v>2.4332833583208302</v>
       </c>
       <c r="M12" s="4">
-        <f>SUM(B12:K12)/10</f>
+        <f t="shared" si="0"/>
         <v>2.3845077461269311</v>
       </c>
       <c r="N12">
-        <f>_xlfn.STDEV.S(B12:K12)</f>
+        <f t="shared" si="1"/>
         <v>0.1059874074020395</v>
       </c>
     </row>
@@ -6328,11 +6501,11 @@
         <v>5.1434256901465396E-4</v>
       </c>
       <c r="M13" s="8">
-        <f>SUM(B13:K13)/10</f>
+        <f t="shared" si="0"/>
         <v>4.5911125611869939E-4</v>
       </c>
       <c r="N13">
-        <f>_xlfn.STDEV.S(B13:K13)</f>
+        <f t="shared" si="1"/>
         <v>4.5179303497271574E-5</v>
       </c>
     </row>
@@ -6371,11 +6544,11 @@
         <v>1.99623939695441E-2</v>
       </c>
       <c r="M14" s="8">
-        <f>SUM(B14:K14)/10</f>
+        <f t="shared" si="0"/>
         <v>1.9167229959915971E-2</v>
       </c>
       <c r="N14">
-        <f>_xlfn.STDEV.S(B14:K14)</f>
+        <f t="shared" si="1"/>
         <v>8.1045269506308274E-4</v>
       </c>
     </row>
@@ -6414,11 +6587,11 @@
         <v>1.5253208317172201E-2</v>
       </c>
       <c r="M15" s="8">
-        <f>SUM(B15:K15)/10</f>
+        <f t="shared" si="0"/>
         <v>1.432999797061249E-2</v>
       </c>
       <c r="N15">
-        <f>_xlfn.STDEV.S(B15:K15)</f>
+        <f t="shared" si="1"/>
         <v>7.498773622832593E-4</v>
       </c>
     </row>
@@ -6457,11 +6630,11 @@
         <v>2.5295536181048499E-5</v>
       </c>
       <c r="M16" s="8">
-        <f>SUM(B16:K16)/10</f>
+        <f t="shared" si="0"/>
         <v>2.4747053833481179E-5</v>
       </c>
       <c r="N16">
-        <f>_xlfn.STDEV.S(B16:K16)</f>
+        <f t="shared" si="1"/>
         <v>1.3958855339595954E-5</v>
       </c>
     </row>
@@ -6500,11 +6673,11 @@
         <v>2.8288841295806E-3</v>
       </c>
       <c r="M17" s="8">
-        <f>SUM(B17:K17)/10</f>
+        <f t="shared" si="0"/>
         <v>2.7101014682564492E-3</v>
       </c>
       <c r="N17">
-        <f>_xlfn.STDEV.S(B17:K17)</f>
+        <f t="shared" si="1"/>
         <v>1.3142271513176995E-4</v>
       </c>
     </row>
@@ -6543,11 +6716,11 @@
         <v>6.2437815140221498E-3</v>
       </c>
       <c r="M18" s="8">
-        <f>SUM(B18:K18)/10</f>
+        <f t="shared" si="0"/>
         <v>5.7613346154347586E-3</v>
       </c>
       <c r="N18">
-        <f>_xlfn.STDEV.S(B18:K18)</f>
+        <f t="shared" si="1"/>
         <v>5.2402096293867133E-4</v>
       </c>
     </row>
@@ -6586,11 +6759,11 @@
         <v>5.2193122986896904E-3</v>
       </c>
       <c r="M19" s="8">
-        <f>SUM(B19:K19)/10</f>
+        <f t="shared" si="0"/>
         <v>5.0055161456185326E-3</v>
       </c>
       <c r="N19">
-        <f>_xlfn.STDEV.S(B19:K19)</f>
+        <f t="shared" si="1"/>
         <v>1.7440362425512939E-4</v>
       </c>
     </row>
@@ -6629,11 +6802,11 @@
         <v>4.6417308892224103E-3</v>
       </c>
       <c r="M20" s="8">
-        <f>SUM(B20:K20)/10</f>
+        <f t="shared" si="0"/>
         <v>4.7784418023759951E-3</v>
       </c>
       <c r="N20">
-        <f>_xlfn.STDEV.S(B20:K20)</f>
+        <f t="shared" si="1"/>
         <v>2.0462267706272607E-4</v>
       </c>
     </row>
@@ -6672,11 +6845,11 @@
         <v>7.9960019990004995E-3</v>
       </c>
       <c r="M21" s="4">
-        <f>SUM(B21:K21)/10</f>
+        <f t="shared" si="0"/>
         <v>6.946526736631679E-3</v>
       </c>
       <c r="N21">
-        <f>_xlfn.STDEV.S(B21:K21)</f>
+        <f t="shared" si="1"/>
         <v>2.2651664065840467E-3</v>
       </c>
     </row>
@@ -6715,11 +6888,11 @@
         <v>0.118940529735132</v>
       </c>
       <c r="M22" s="4">
-        <f>SUM(B22:K22)/10</f>
+        <f t="shared" si="0"/>
         <v>0.18190904547726083</v>
       </c>
       <c r="N22">
-        <f>_xlfn.STDEV.S(B22:K22)</f>
+        <f t="shared" si="1"/>
         <v>3.0706517344097569E-2</v>
       </c>
     </row>

</xml_diff>